<commit_message>
trying to fix scaling
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Bild</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>mmpi</t>
+  </si>
+  <si>
+    <t>wA4</t>
   </si>
 </sst>
 </file>
@@ -469,6 +472,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
       <c r="B9">
         <f>B6-B7-B8</f>
         <v>210</v>

</xml_diff>